<commit_message>
se agrega procesamiento para variables al cuadrado
</commit_message>
<xml_diff>
--- a/test/test_inputs/Modelos_test.xlsx
+++ b/test/test_inputs/Modelos_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Trabajo\2022 - Demanda Electrica Coordinador\App\test\test_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AE48E0-0AA1-4EF6-9BE4-414B722D224B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F6A6E3-D636-4FAD-A1F6-C6769720C4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuracion" sheetId="14" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="EFMes_ReguladosLD_1" sheetId="13" r:id="rId3"/>
     <sheet name="EF_ReguladosLD_1" sheetId="1" r:id="rId4"/>
     <sheet name="Var_ReguladosLD_1" sheetId="7" r:id="rId5"/>
-    <sheet name="EF_ReguladosLD_2" sheetId="5" r:id="rId6"/>
-    <sheet name="EF_ReguladosLD_3" sheetId="6" r:id="rId7"/>
-    <sheet name="ReguladosLD_Var_3" sheetId="9" r:id="rId8"/>
-    <sheet name="EF_Cobre_1" sheetId="2" r:id="rId9"/>
-    <sheet name="Var_Cobre_1" sheetId="15" r:id="rId10"/>
-    <sheet name="Var_ReguladosLD_2" sheetId="8" r:id="rId11"/>
-    <sheet name="Desagregacion_Comuna" sheetId="4" r:id="rId12"/>
-    <sheet name="Desagregacion_Empresa" sheetId="10" r:id="rId13"/>
-    <sheet name="Asignacion_Barra" sheetId="12" r:id="rId14"/>
+    <sheet name="Var2_ReguladosLD_1" sheetId="16" r:id="rId6"/>
+    <sheet name="EF_ReguladosLD_2" sheetId="5" r:id="rId7"/>
+    <sheet name="EF_ReguladosLD_3" sheetId="6" r:id="rId8"/>
+    <sheet name="ReguladosLD_Var_3" sheetId="9" r:id="rId9"/>
+    <sheet name="EF_Cobre_1" sheetId="2" r:id="rId10"/>
+    <sheet name="Var_Cobre_1" sheetId="15" r:id="rId11"/>
+    <sheet name="Var_ReguladosLD_2" sheetId="8" r:id="rId12"/>
+    <sheet name="Desagregacion_Comuna" sheetId="4" r:id="rId13"/>
+    <sheet name="Desagregacion_Empresa" sheetId="10" r:id="rId14"/>
+    <sheet name="Asignacion_Barra" sheetId="12" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="571">
   <si>
     <t>Comuna</t>
   </si>
@@ -2103,7 +2104,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2142,6 +2143,64 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4676126E-1C18-4B0A-8449-E38C53E07C6E}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC2696B-20E8-4ABD-91B3-7614E836A1BE}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2172,7 +2231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D1459-E4D9-4CB5-9158-1D2F087C234F}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -2242,7 +2301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5302D3BC-B920-4C03-9052-ADF26D9DBF18}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
@@ -2296,7 +2355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4389CED-6485-43A3-85B4-8F5911919B0E}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
@@ -2347,7 +2406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383DD44E-FD1E-48BC-A4C3-80BA76339FF8}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
@@ -2397,7 +2456,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2667,8 +2726,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,6 +2770,37 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AA906D-241E-4666-A826-DA21D34EFA7D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE73B2E-EBDC-4862-A71B-5CF4255979CD}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -6910,7 +7000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6F29D8-5E28-43CF-83F3-0EB79EE19EC1}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -38355,7 +38445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C73DA3-F775-4235-B645-9FF014AD32B7}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -38653,62 +38743,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4676126E-1C18-4B0A-8449-E38C53E07C6E}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
se agrega test para coeficientes cuadrados
</commit_message>
<xml_diff>
--- a/test/test_inputs/Modelos_test.xlsx
+++ b/test/test_inputs/Modelos_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Trabajo\2022 - Demanda Electrica Coordinador\App\test\test_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F6A6E3-D636-4FAD-A1F6-C6769720C4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346FABC3-668A-4142-A415-24E356694FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2104,7 +2104,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,7 +2774,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>